<commit_message>
Excel Group import automatically enables Web Hook Results reporting for Individual Groups
Any group not matching a 32-character hex Group Title will be disabled for reporting.

CVDLS-220
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6CB3CC-14AB-CF48-A5C3-B22AD901E185}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3701B4-0B67-8949-A5E1-7197FC9A7A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="460" windowWidth="15320" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
+    <workbookView xWindow="8740" yWindow="460" windowWidth="17920" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Not Used</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>SN4</t>
+  </si>
+  <si>
+    <t>09876543210987654321abcdefABCDEF</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,6 +556,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="D10" s="3"/>

</xml_diff>

<commit_message>
Participant Group Excel Import parses flag for enabling Web Hooks
Column L in Excel must use values 0 or 1.

CVDLS-220
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3701B4-0B67-8949-A5E1-7197FC9A7A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E05EBE-1196-CB4A-BFFA-FB851E8C692C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8740" yWindow="460" windowWidth="17920" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
+    <workbookView xWindow="3980" yWindow="460" windowWidth="22680" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Not Used</t>
   </si>
@@ -72,30 +72,19 @@
   </si>
   <si>
     <t>09876543210987654321abcdefABCDEF</t>
+  </si>
+  <si>
+    <t>Enable Web Hooks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,17 +105,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,19 +122,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBBEC93-7333-1442-B72C-828450A2C003}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,41 +459,45 @@
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
     <col min="6" max="7" width="12.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -522,8 +507,11 @@
       <c r="J2" t="s">
         <v>5</v>
       </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>9</v>
       </c>
@@ -533,8 +521,11 @@
       <c r="J3" t="s">
         <v>6</v>
       </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -544,8 +535,11 @@
       <c r="J5" t="s">
         <v>7</v>
       </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -555,8 +549,11 @@
       <c r="J6" t="s">
         <v>8</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>12</v>
       </c>
@@ -566,13 +563,17 @@
       <c r="J7" t="s">
         <v>12</v>
       </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-      <c r="D10" s="3"/>
-    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Participant Group Excel Import properly validates empty Participant Count
CVDLS-220
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E05EBE-1196-CB4A-BFFA-FB851E8C692C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C665DCEA-5FA2-ED46-8BE9-DA9D4763CB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="460" windowWidth="22680" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Not Used</t>
   </si>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>Enable Web Hooks</t>
+  </si>
+  <si>
+    <t>09876543210987654322abcdefABCDEF</t>
+  </si>
+  <si>
+    <t>09876543210987654323abcdefABCDEF</t>
+  </si>
+  <si>
+    <t>09876543210987654324abcdefABCDEF</t>
+  </si>
+  <si>
+    <t>09876543210987654325abcdefABCDEF</t>
+  </si>
+  <si>
+    <t>09876543210987654326abcdefABCDEF</t>
+  </si>
+  <si>
+    <t>WRONG VALUE</t>
   </si>
 </sst>
 </file>
@@ -105,12 +123,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,10 +149,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -447,7 +472,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,11 +592,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C8" s="3"/>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Participant Group Import supports true / false boolean in Enable Web Hooks column
CVDLS-220
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C665DCEA-5FA2-ED46-8BE9-DA9D4763CB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156E71CF-549A-E245-8ED3-73C9E2DB6171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="460" windowWidth="22680" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
@@ -532,7 +532,7 @@
       <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -546,7 +546,7 @@
       <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="L3">
+      <c r="L3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -560,7 +560,7 @@
       <c r="J5" t="s">
         <v>7</v>
       </c>
-      <c r="L5">
+      <c r="L5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -574,7 +574,7 @@
       <c r="J6" t="s">
         <v>8</v>
       </c>
-      <c r="L6">
+      <c r="L6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -588,7 +588,7 @@
       <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="L7">
+      <c r="L7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -600,7 +600,7 @@
       <c r="J8" t="s">
         <v>14</v>
       </c>
-      <c r="L8">
+      <c r="L8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -612,7 +612,7 @@
       <c r="J9" t="s">
         <v>15</v>
       </c>
-      <c r="L9">
+      <c r="L9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="3"/>
-      <c r="L10">
+      <c r="L10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Group Import temporarily allows empty values for Column L used for Enable Web Hooks
Will default to NO, which is what we want

CVDLS-220
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156E71CF-549A-E245-8ED3-73C9E2DB6171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F6E67C-6752-7E40-85B3-D9A0600DE1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="460" windowWidth="22680" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Not Used</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>WRONG VALUE</t>
+  </si>
+  <si>
+    <t>CHANGE BACK TO EMPTY</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,12 +158,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +482,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,6 +494,7 @@
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
     <col min="6" max="7" width="12.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -546,9 +557,7 @@
       <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
+      <c r="L3" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
@@ -638,7 +647,9 @@
       <c r="J11" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" t="s">

</xml_diff>

<commit_message>
Participant Group Import honors Column K for Is Active status
Prior to this commit all imported groups were made Active.

After this commit the TRUE or FALSE value in Column K represents that Active status.

CVDLS-213
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F6E67C-6752-7E40-85B3-D9A0600DE1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B59CF4-DBF7-8742-BCA1-DF891F2D68A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="460" windowWidth="22680" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
+    <workbookView xWindow="4600" yWindow="460" windowWidth="24120" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Not Used</t>
   </si>
@@ -96,6 +96,27 @@
   </si>
   <si>
     <t>CHANGE BACK TO EMPTY</t>
+  </si>
+  <si>
+    <t>Is Active?</t>
+  </si>
+  <si>
+    <t>SN5</t>
+  </si>
+  <si>
+    <t>Fifth</t>
+  </si>
+  <si>
+    <t>SN6</t>
+  </si>
+  <si>
+    <t>Sixth</t>
+  </si>
+  <si>
+    <t>Seventh</t>
+  </si>
+  <si>
+    <t>SN7</t>
   </si>
 </sst>
 </file>
@@ -479,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBBEC93-7333-1442-B72C-828450A2C003}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,7 +516,7 @@
     <col min="6" max="7" width="12.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" customWidth="1"/>
     <col min="11" max="11" width="22.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -529,6 +550,9 @@
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
@@ -543,6 +567,9 @@
       <c r="J2" t="s">
         <v>5</v>
       </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
       <c r="L2" t="b">
         <v>0</v>
       </c>
@@ -557,6 +584,9 @@
       <c r="J3" t="s">
         <v>6</v>
       </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
       <c r="L3" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -569,6 +599,9 @@
       <c r="J5" t="s">
         <v>7</v>
       </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
       <c r="L5" t="b">
         <v>0</v>
       </c>
@@ -583,6 +616,9 @@
       <c r="J6" t="s">
         <v>8</v>
       </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
       <c r="L6" t="b">
         <v>0</v>
       </c>
@@ -597,6 +633,9 @@
       <c r="J7" t="s">
         <v>12</v>
       </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
       <c r="L7" t="b">
         <v>1</v>
       </c>
@@ -609,6 +648,9 @@
       <c r="J8" t="s">
         <v>14</v>
       </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
       <c r="L8" t="b">
         <v>1</v>
       </c>
@@ -621,6 +663,9 @@
       <c r="J9" t="s">
         <v>15</v>
       </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
       <c r="L9" t="b">
         <v>1</v>
       </c>
@@ -633,6 +678,9 @@
         <v>1</v>
       </c>
       <c r="J10" s="3"/>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
       <c r="L10" t="b">
         <v>1</v>
       </c>
@@ -647,6 +695,9 @@
       <c r="J11" t="s">
         <v>17</v>
       </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
       <c r="L11" s="3" t="s">
         <v>20</v>
       </c>
@@ -661,8 +712,60 @@
       <c r="J12" t="s">
         <v>18</v>
       </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
       <c r="L12" s="3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <v>9</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
viralResultsWebHooksEnabled and antibodyResultsWebHooksEnabled replace entity field ParticipantGroup.enabledForResultsWebHooks
Old field enabledForResultsWebHooks was split into 2 in previous commits.
This commit does the real replacement and removes all traces of enabledForResultsWebHooks.

Future work will allow Participant Group Import to change these new flags via Excel, and provide form UI to update them.

enabledForResultsWebHooks will remain in ParticipantGroup audit log records so
the entity must still read it for parsing logs.

CVDLS-227
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B59CF4-DBF7-8742-BCA1-DF891F2D68A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A21EC56-F652-CD4C-826B-4279EFBD8FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4600" yWindow="460" windowWidth="24120" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Not Used</t>
   </si>
@@ -74,9 +74,6 @@
     <t>09876543210987654321abcdefABCDEF</t>
   </si>
   <si>
-    <t>Enable Web Hooks</t>
-  </si>
-  <si>
     <t>09876543210987654322abcdefABCDEF</t>
   </si>
   <si>
@@ -86,16 +83,7 @@
     <t>09876543210987654324abcdefABCDEF</t>
   </si>
   <si>
-    <t>09876543210987654325abcdefABCDEF</t>
-  </si>
-  <si>
-    <t>09876543210987654326abcdefABCDEF</t>
-  </si>
-  <si>
     <t>WRONG VALUE</t>
-  </si>
-  <si>
-    <t>CHANGE BACK TO EMPTY</t>
   </si>
   <si>
     <t>Is Active?</t>
@@ -147,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,12 +145,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBBEC93-7333-1442-B72C-828450A2C003}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,7 +498,7 @@
     <col min="6" max="7" width="12.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" customWidth="1"/>
     <col min="11" max="11" width="22.6640625" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -551,11 +533,9 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
@@ -570,9 +550,7 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
@@ -587,7 +565,10 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
@@ -602,9 +583,7 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
@@ -619,9 +598,7 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-      <c r="L6" t="b">
-        <v>0</v>
-      </c>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
@@ -636,9 +613,7 @@
       <c r="K7" t="b">
         <v>1</v>
       </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C8" s="3"/>
@@ -646,33 +621,29 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" t="b">
         <v>1</v>
       </c>
-      <c r="L8" t="b">
-        <v>1</v>
-      </c>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="3"/>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K9" t="b">
         <v>1</v>
       </c>
-      <c r="L9" t="b">
-        <v>1</v>
-      </c>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
@@ -681,92 +652,58 @@
       <c r="K10" t="b">
         <v>1</v>
       </c>
-      <c r="L10" t="b">
-        <v>1</v>
-      </c>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" t="b">
-        <v>1</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="H11" s="4"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="H12" s="4"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H13">
         <v>8</v>
       </c>
       <c r="J13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
       </c>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H14">
         <v>9</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K14" s="3"/>
-      <c r="L14" t="b">
-        <v>0</v>
-      </c>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" t="b">
-        <v>0</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="L15" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Participant Group re-maps columns to latest ServiceNow export
Introduces new columns:
- Accept Saliva?
- Accept Blood?
- Viral Web Hooks Enabled?
- Antibody Web Hooks Enabled?

CVDLS-227
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A21EC56-F652-CD4C-826B-4279EFBD8FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D53B85-205B-5A45-B358-9E26F2790AD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="460" windowWidth="24120" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
+    <workbookView xWindow="14000" yWindow="460" windowWidth="23580" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
-  <si>
-    <t>Not Used</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>ServiceNow ID</t>
   </si>
@@ -105,6 +102,66 @@
   </si>
   <si>
     <t>SN7</t>
+  </si>
+  <si>
+    <t>Accept Saliva</t>
+  </si>
+  <si>
+    <t>Accept Blood</t>
+  </si>
+  <si>
+    <t>Saliva Web Hooks</t>
+  </si>
+  <si>
+    <t>Blood Web Hooks</t>
+  </si>
+  <si>
+    <t>Group100</t>
+  </si>
+  <si>
+    <t>Group101</t>
+  </si>
+  <si>
+    <t>Group102</t>
+  </si>
+  <si>
+    <t>Group103</t>
+  </si>
+  <si>
+    <t>Group104</t>
+  </si>
+  <si>
+    <t>Group105</t>
+  </si>
+  <si>
+    <t>Group106</t>
+  </si>
+  <si>
+    <t>Group107</t>
+  </si>
+  <si>
+    <t>SN100</t>
+  </si>
+  <si>
+    <t>SN101</t>
+  </si>
+  <si>
+    <t>SN102</t>
+  </si>
+  <si>
+    <t>SN103</t>
+  </si>
+  <si>
+    <t>SN104</t>
+  </si>
+  <si>
+    <t>SN105</t>
+  </si>
+  <si>
+    <t>SN106</t>
+  </si>
+  <si>
+    <t>SN107</t>
   </si>
 </sst>
 </file>
@@ -161,10 +218,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -482,228 +538,561 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBBEC93-7333-1442-B72C-828450A2C003}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="7" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.6640625" customWidth="1"/>
     <col min="12" max="12" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
         <v>9</v>
       </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
         <v>10</v>
       </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
         <v>8</v>
       </c>
-      <c r="K6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C8" s="3"/>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="J9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="4">
-        <v>1</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" t="b">
-        <v>1</v>
-      </c>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H11" s="4"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H12" s="4"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13">
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18">
         <v>8</v>
       </c>
-      <c r="J13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14">
-        <v>9</v>
-      </c>
-      <c r="J14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" s="4"/>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="L24" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Group Import prevents duplicate Title and External ID values in same import
Displays user-visible error message

CVDLS-227
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D53B85-205B-5A45-B358-9E26F2790AD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC19EFE-5C24-3B46-8B42-4EC7F0885105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="460" windowWidth="23580" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
+    <workbookView xWindow="5220" yWindow="460" windowWidth="23580" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>ServiceNow ID</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>SN107</t>
+  </si>
+  <si>
+    <t>SN2222</t>
+  </si>
+  <si>
+    <t>Eighth</t>
   </si>
 </sst>
 </file>
@@ -538,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBBEC93-7333-1442-B72C-828450A2C003}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1094,6 +1100,58 @@
       <c r="I24" s="2"/>
       <c r="L24" s="3"/>
     </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Group import now allows duplicate External IDs
The external system is not our concern. If they don't want duplicates they should remove them.
This might allow for multiple external systems that use the same identifier.

CVDLS-227
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
+++ b/tests/ExcelImport/workbooks/participant-group-importer-new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC19EFE-5C24-3B46-8B42-4EC7F0885105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F76ECE4-85FB-D646-8F95-B2522421002A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="460" windowWidth="23580" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>ServiceNow ID</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>SN2222</t>
-  </si>
-  <si>
-    <t>Eighth</t>
   </si>
 </sst>
 </file>
@@ -547,12 +544,12 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
@@ -734,7 +731,7 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3"/>
       <c r="D8">
         <v>1</v>
       </c>
@@ -1127,30 +1124,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" t="b">
-        <v>0</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>